<commit_message>
More cold start chart
</commit_message>
<xml_diff>
--- a/src/documents/2018/04/azure-functions-cold-starts-in-numbers/AzureColdStarts.xlsx
+++ b/src/documents/2018/04/azure-functions-cold-starts-in-numbers/AzureColdStarts.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20325"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\mikhailio-docpad\src\documents\2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Work\mikhailio-docpad\src\documents\2018\04\azure-functions-cold-starts-in-numbers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A6CE808C-A1CB-45EE-95B7-E7435A66A74D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE52CED5-B208-46DC-A35C-F2B0875A7402}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24686" windowHeight="9617" activeTab="1" xr2:uid="{F8F11C14-CDC6-4AC8-A8A4-A6434409164B}"/>
   </bookViews>
@@ -20,10 +20,15 @@
     <sheet name="cs-v2" sheetId="5" r:id="rId5"/>
     <sheet name="mixed" sheetId="6" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="179021"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -2768,10 +2773,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B319610E-AF17-4981-8D1C-4CCC62115A31}">
-  <dimension ref="A1:H52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="K52" sqref="K52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -3977,7 +3982,7 @@
         <v>2049</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A49" s="1">
         <v>43210.801427604165</v>
       </c>
@@ -4003,7 +4008,7 @@
         <v>1897</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A50" s="1">
         <v>43210.823644942131</v>
       </c>
@@ -4029,7 +4034,7 @@
         <v>2042</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.4">
       <c r="A51" s="1">
         <v>43210.840316423608</v>
       </c>
@@ -4049,9 +4054,29 @@
         <v>2751</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.4">
       <c r="B52">
         <f>MAX(B2:B51)</f>
+        <v>5808</v>
+      </c>
+      <c r="H52">
+        <f>MIN($H4:$H51)</f>
+        <v>1484</v>
+      </c>
+      <c r="I52">
+        <f>PERCENTILE($H4:$H51,0.18)</f>
+        <v>1858.6</v>
+      </c>
+      <c r="J52">
+        <f>PERCENTILE($H4:$H51,0.82)</f>
+        <v>2448</v>
+      </c>
+      <c r="K52">
+        <f>PERCENTILE($H4:$H51,0.975)</f>
+        <v>3876</v>
+      </c>
+      <c r="L52">
+        <f>MAX($H4:$H51)</f>
         <v>5808</v>
       </c>
     </row>
@@ -4068,8 +4093,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BDA42E33-57C2-4602-B158-590FF84B8FDD}">
   <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="L51" sqref="H51:L51"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -5350,16 +5375,16 @@
         <v>1189</v>
       </c>
       <c r="I51">
-        <f>PERCENTILE($H3:$H50,0.25)</f>
-        <v>1739</v>
+        <f>PERCENTILE($H3:$H50,0.18)</f>
+        <v>1578.3999999999999</v>
       </c>
       <c r="J51">
         <f>PERCENTILE($H3:$H50,0.5)</f>
         <v>2061</v>
       </c>
       <c r="K51">
-        <f>PERCENTILE($H3:$H50,0.75)</f>
-        <v>2346</v>
+        <f>PERCENTILE($H3:$H50,0.975)</f>
+        <v>5462</v>
       </c>
       <c r="L51">
         <f>MAX($H3:$H50)</f>

</xml_diff>